<commit_message>
After correcting all of the SEPT10 errors in primary and master data files.
</commit_message>
<xml_diff>
--- a/comp_avail_needed.xlsx
+++ b/comp_avail_needed.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="17820" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="17820" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="prefrontal" sheetId="1" r:id="rId1"/>
+    <sheet name="prefrontal" sheetId="6" r:id="rId1"/>
     <sheet name="cerebellum" sheetId="2" r:id="rId2"/>
     <sheet name="temporal" sheetId="5" r:id="rId3"/>
     <sheet name="pons" sheetId="4" r:id="rId4"/>
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="comp_avail_needed_cerebellum" localSheetId="1">cerebellum!$A$1:$H$41</definedName>
     <definedName name="comp_avail_needed_pons" localSheetId="3">pons!$A$1:$H$48</definedName>
-    <definedName name="comp_avail_needed_prefrontal" localSheetId="0">prefrontal!$A$1:$H$43</definedName>
+    <definedName name="comp_avail_needed_prefrontal" localSheetId="0">prefrontal!$A$1:$H$48</definedName>
     <definedName name="comp_avail_needed_temporal" localSheetId="2">temporal!$A$1:$H$49</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -71,7 +71,21 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="comp_avail_needed_temporal.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" name="comp_avail_needed_prefrontal.txt1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh_HD_3:genetics:genenetwork2:comp_avail_needed_prefrontal.txt" tab="0" comma="1">
+      <textFields count="8">
+        <textField/>
+        <textField/>
+        <textField type="text"/>
+        <textField type="text"/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="comp_avail_needed_temporal.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh_HD_3:genetics:genenetwork2:comp_avail_needed_temporal.txt" tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -85,7 +99,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="comp_avail_needed_temporal.txt1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="6" name="comp_avail_needed_temporal.txt1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh_HD_3:genetics:genenetwork2:comp_avail_needed_temporal.txt" tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -103,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="95">
   <si>
     <t>r.entrez</t>
   </si>
@@ -141,9 +155,6 @@
     <t>ACTR3C</t>
   </si>
   <si>
-    <t>FAM27E2</t>
-  </si>
-  <si>
     <t>ERVK13-1</t>
   </si>
   <si>
@@ -249,9 +260,6 @@
     <t>DEFB4B</t>
   </si>
   <si>
-    <t>IGHV5-78</t>
-  </si>
-  <si>
     <t>RRN3P1</t>
   </si>
   <si>
@@ -373,6 +381,27 @@
   </si>
   <si>
     <t>C10orf71</t>
+  </si>
+  <si>
+    <t>LOC401622</t>
+  </si>
+  <si>
+    <t>ZNF391</t>
+  </si>
+  <si>
+    <t>LOC441179</t>
+  </si>
+  <si>
+    <t>ASAH2B</t>
+  </si>
+  <si>
+    <t>LOC653501</t>
+  </si>
+  <si>
+    <t>CCR5</t>
+  </si>
+  <si>
+    <t>COL23A1</t>
   </si>
 </sst>
 </file>
@@ -421,7 +450,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="comp_avail_needed_prefrontal" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="comp_avail_needed_prefrontal" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -429,7 +458,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="comp_avail_needed_temporal" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="comp_avail_needed_temporal" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -758,9 +787,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0"/>
   <cols>
@@ -799,88 +828,88 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>115648</v>
+        <v>143188</v>
       </c>
       <c r="B2">
-        <v>115648</v>
+        <v>143188</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>114.61067199999999</v>
       </c>
       <c r="H2">
-        <v>21.382659</v>
+        <v>114.61067199999999</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>143188</v>
+        <v>65385</v>
       </c>
       <c r="B3">
-        <v>143188</v>
+        <v>65385</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G3">
-        <v>114.61067199999999</v>
+        <v>149.881359</v>
       </c>
       <c r="H3">
-        <v>114.61067199999999</v>
+        <v>149.881359</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>155060</v>
+        <v>100289124</v>
       </c>
       <c r="B4">
-        <v>155060</v>
+        <v>100289124</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G4">
-        <v>149.28528</v>
+        <v>41.647674000000002</v>
       </c>
       <c r="H4">
-        <v>149.28528</v>
+        <v>41.647674000000002</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>504188</v>
+        <v>100507321</v>
       </c>
       <c r="B5">
-        <v>504188</v>
+        <v>100507321</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -889,134 +918,134 @@
         <v>12</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G5">
-        <v>45.623565999999997</v>
+        <v>2.6583890000000001</v>
       </c>
       <c r="H5">
-        <v>45.623565999999997</v>
+        <v>2.6583890000000001</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
-        <v>283874</v>
+        <v>284009</v>
       </c>
       <c r="B6">
-        <v>283874</v>
+        <v>284009</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="E6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6">
-        <v>2.6511499999999999</v>
+        <v>2.4069799999999999</v>
       </c>
       <c r="H6">
-        <v>2.6511499999999999</v>
+        <v>2.4069799999999999</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
-        <v>284912</v>
+        <v>85452</v>
       </c>
       <c r="B7">
-        <v>284912</v>
+        <v>85452</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="E7">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>35.627575</v>
+        <v>1.921951</v>
       </c>
       <c r="H7">
-        <v>35.627575</v>
+        <v>1.921951</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
-        <v>282808</v>
+        <v>8027</v>
       </c>
       <c r="B8">
-        <v>282808</v>
+        <v>8027</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
+        <v>71</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
       </c>
       <c r="G8">
-        <v>102.93727199999999</v>
+        <v>17.644124999999999</v>
       </c>
       <c r="H8">
-        <v>102.93727199999999</v>
+        <v>17.644124999999999</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
-        <v>2782</v>
+        <v>387720</v>
       </c>
       <c r="B9">
-        <v>2782</v>
+        <v>387720</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G9">
-        <v>1.785285</v>
+        <v>127.73460900000001</v>
       </c>
       <c r="H9">
-        <v>1.785285</v>
+        <v>127.73460900000001</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
-        <v>387820</v>
+        <v>100506127</v>
       </c>
       <c r="B10">
-        <v>387820</v>
+        <v>100506127</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="E10">
         <v>11</v>
@@ -1025,76 +1054,76 @@
         <v>11</v>
       </c>
       <c r="G10">
-        <v>127.940983</v>
+        <v>76.381303000000003</v>
       </c>
       <c r="H10">
-        <v>127.940983</v>
+        <v>76.381303000000003</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
-        <v>728524</v>
+        <v>2113</v>
       </c>
       <c r="B11">
-        <v>728524</v>
+        <v>2113</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G11">
-        <v>73.019730999999993</v>
+        <v>128.45876100000001</v>
       </c>
       <c r="H11">
-        <v>73.019730999999993</v>
+        <v>128.45876100000001</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12">
-        <v>389833</v>
+        <v>388022</v>
       </c>
       <c r="B12">
-        <v>389833</v>
+        <v>388022</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F12">
-        <v>4</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>104.719759</v>
       </c>
       <c r="H12">
-        <v>2.6502000000000001E-2</v>
+        <v>104.719759</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13">
-        <v>256158</v>
+        <v>392395</v>
       </c>
       <c r="B13">
-        <v>256158</v>
+        <v>392395</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="E13">
         <v>9</v>
@@ -1102,19 +1131,19 @@
       <c r="F13">
         <v>9</v>
       </c>
-      <c r="G13">
-        <v>130.26574199999999</v>
-      </c>
-      <c r="H13">
-        <v>130.26574199999999</v>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14">
-        <v>399900</v>
+        <v>400499</v>
       </c>
       <c r="B14">
-        <v>399900</v>
+        <v>400499</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>22</v>
@@ -1123,56 +1152,56 @@
         <v>22</v>
       </c>
       <c r="E14">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F14">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G14">
-        <v>61.967796999999997</v>
+        <v>11.372014</v>
       </c>
       <c r="H14">
-        <v>61.967796999999997</v>
+        <v>11.372014</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15">
-        <v>400499</v>
+        <v>400924</v>
       </c>
       <c r="B15">
-        <v>400499</v>
+        <v>400924</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="E15">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F15">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G15">
-        <v>11.372014</v>
+        <v>28.756105999999999</v>
       </c>
       <c r="H15">
-        <v>11.372014</v>
+        <v>28.756105999999999</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16">
-        <v>401052</v>
+        <v>442075</v>
       </c>
       <c r="B16">
-        <v>401052</v>
+        <v>442075</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -1181,18 +1210,18 @@
         <v>3</v>
       </c>
       <c r="G16">
-        <v>10.006417000000001</v>
+        <v>9.9868930000000002</v>
       </c>
       <c r="H16">
-        <v>10.006417000000001</v>
+        <v>9.9868930000000002</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
-        <v>401252</v>
+        <v>401296</v>
       </c>
       <c r="B17">
-        <v>401252</v>
+        <v>401296</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
@@ -1201,30 +1230,30 @@
         <v>25</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G17">
-        <v>32.331465000000001</v>
+        <v>1.690812</v>
       </c>
       <c r="H17">
-        <v>32.331465000000001</v>
+        <v>1.690812</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
-        <v>401296</v>
+        <v>55750</v>
       </c>
       <c r="B18">
-        <v>401296</v>
+        <v>55750</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="E18">
         <v>7</v>
@@ -1233,18 +1262,18 @@
         <v>7</v>
       </c>
       <c r="G18">
-        <v>1.690812</v>
+        <v>141.551278</v>
       </c>
       <c r="H18">
-        <v>1.690812</v>
+        <v>141.551278</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19">
-        <v>401357</v>
+        <v>401433</v>
       </c>
       <c r="B19">
-        <v>401357</v>
+        <v>401433</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>27</v>
@@ -1259,36 +1288,36 @@
         <v>7</v>
       </c>
       <c r="G19">
-        <v>56.809123</v>
+        <v>151.07413</v>
       </c>
       <c r="H19">
-        <v>56.809123</v>
+        <v>151.07413</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20">
-        <v>401433</v>
+        <v>401589</v>
       </c>
       <c r="B20">
-        <v>401433</v>
+        <v>401589</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20">
-        <v>7</v>
-      </c>
-      <c r="F20">
-        <v>7</v>
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
       </c>
       <c r="G20">
-        <v>151.07413</v>
+        <v>52.051169999999999</v>
       </c>
       <c r="H20">
-        <v>151.07413</v>
+        <v>52.051169999999999</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1299,19 +1328,19 @@
         <v>401620</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <v>151.01788400000001</v>
       </c>
       <c r="H21">
         <v>151.01788400000001</v>
@@ -1319,42 +1348,42 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22">
-        <v>440258</v>
+        <v>401622</v>
       </c>
       <c r="B22">
-        <v>440258</v>
+        <v>401622</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22">
-        <v>8</v>
-      </c>
-      <c r="F22">
-        <v>8</v>
-      </c>
-      <c r="G22" t="s">
-        <v>9</v>
+        <v>88</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22">
+        <v>154.23794799999999</v>
       </c>
       <c r="H22">
-        <v>26.308713999999998</v>
+        <v>154.23794799999999</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23">
-        <v>440570</v>
+        <v>23400</v>
       </c>
       <c r="B23">
-        <v>440570</v>
+        <v>23400</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1362,11 +1391,11 @@
       <c r="F23">
         <v>1</v>
       </c>
-      <c r="G23" t="s">
-        <v>9</v>
+      <c r="G23">
+        <v>16.985958</v>
       </c>
       <c r="H23">
-        <v>17.071733999999999</v>
+        <v>16.985958</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1377,10 +1406,10 @@
         <v>441120</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E24">
         <v>5</v>
@@ -1388,8 +1417,8 @@
       <c r="F24">
         <v>5</v>
       </c>
-      <c r="G24" t="s">
-        <v>9</v>
+      <c r="G24">
+        <v>179.01233099999999</v>
       </c>
       <c r="H24">
         <v>179.01233099999999</v>
@@ -1397,120 +1426,120 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25">
-        <v>441193</v>
+        <v>346157</v>
       </c>
       <c r="B25">
-        <v>441193</v>
+        <v>346157</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="E25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <v>5.426139</v>
+        <v>27.374635000000001</v>
       </c>
       <c r="H25">
-        <v>5.426139</v>
+        <v>27.374635000000001</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26">
-        <v>441257</v>
+        <v>441179</v>
       </c>
       <c r="B26">
-        <v>441257</v>
+        <v>441179</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="E26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26">
-        <v>7</v>
-      </c>
-      <c r="G26" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>167.79552799999999</v>
       </c>
       <c r="H26">
-        <v>72.134118000000001</v>
+        <v>167.79552799999999</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27">
-        <v>441956</v>
+        <v>441193</v>
       </c>
       <c r="B27">
-        <v>441956</v>
+        <v>441193</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E27">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F27">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="G27">
-        <v>13.679218000000001</v>
+        <v>5.426139</v>
       </c>
       <c r="H27">
-        <v>13.679218000000001</v>
+        <v>5.426139</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28">
-        <v>100289124</v>
+        <v>441233</v>
       </c>
       <c r="B28">
-        <v>100289124</v>
+        <v>441233</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="E28">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F28">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G28">
-        <v>41.647674000000002</v>
+        <v>57.475796000000003</v>
       </c>
       <c r="H28">
-        <v>41.647674000000002</v>
+        <v>57.475796000000003</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29">
-        <v>541473</v>
+        <v>441257</v>
       </c>
       <c r="B29">
-        <v>541473</v>
+        <v>441257</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E29">
         <v>7</v>
@@ -1519,206 +1548,206 @@
         <v>7</v>
       </c>
       <c r="G29">
-        <v>75.391947999999999</v>
+        <v>72.134118000000001</v>
       </c>
       <c r="H29">
-        <v>75.391947999999999</v>
+        <v>72.134118000000001</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30">
-        <v>613266</v>
+        <v>441956</v>
       </c>
       <c r="B30">
-        <v>613266</v>
+        <v>441956</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E30">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F30">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G30">
-        <v>15.892332</v>
+        <v>13.679218000000001</v>
       </c>
       <c r="H30">
-        <v>15.892332</v>
+        <v>13.679218000000001</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31">
-        <v>644563</v>
+        <v>541473</v>
       </c>
       <c r="B31">
-        <v>644563</v>
+        <v>541473</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" t="s">
-        <v>16</v>
+        <v>35</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>7</v>
       </c>
       <c r="G31">
-        <v>107.131573</v>
+        <v>75.391947999999999</v>
       </c>
       <c r="H31">
-        <v>107.131573</v>
+        <v>75.391947999999999</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32">
-        <v>646347</v>
+        <v>23325</v>
       </c>
       <c r="B32">
-        <v>646347</v>
+        <v>23325</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G32">
-        <v>160.89488800000001</v>
+        <v>105.107714</v>
       </c>
       <c r="H32">
-        <v>160.89488800000001</v>
+        <v>105.107714</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33">
-        <v>646434</v>
+        <v>644563</v>
       </c>
       <c r="B33">
-        <v>646434</v>
+        <v>644563</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33">
-        <v>10</v>
-      </c>
-      <c r="F33">
-        <v>10</v>
-      </c>
-      <c r="G33" t="s">
-        <v>9</v>
+        <v>37</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33">
+        <v>107.131573</v>
       </c>
       <c r="H33">
-        <v>38.776983000000001</v>
+        <v>107.131573</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34">
-        <v>646517</v>
+        <v>646347</v>
       </c>
       <c r="B34">
-        <v>646517</v>
+        <v>646347</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E34">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F34">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G34">
-        <v>51.409883000000001</v>
+        <v>160.89488800000001</v>
       </c>
       <c r="H34">
-        <v>51.409883000000001</v>
+        <v>160.89488800000001</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35">
-        <v>647115</v>
+        <v>399744</v>
       </c>
       <c r="B35">
-        <v>647115</v>
+        <v>399744</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G35">
-        <v>63.841106000000003</v>
+        <v>38.428145999999998</v>
       </c>
       <c r="H35">
-        <v>63.841106000000003</v>
+        <v>38.428145999999998</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" t="s">
-        <v>9</v>
+      <c r="A36">
+        <v>646517</v>
+      </c>
+      <c r="B36">
+        <v>646517</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" t="s">
-        <v>9</v>
-      </c>
-      <c r="H36" t="s">
-        <v>9</v>
+        <v>40</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+      <c r="G36">
+        <v>51.409883000000001</v>
+      </c>
+      <c r="H36">
+        <v>51.409883000000001</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37">
-        <v>727726</v>
+        <v>653308</v>
       </c>
       <c r="B37">
-        <v>727726</v>
+        <v>653308</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="E37">
         <v>10</v>
@@ -1727,166 +1756,296 @@
         <v>10</v>
       </c>
       <c r="G37">
-        <v>50.696330000000003</v>
+        <v>50.739688000000001</v>
       </c>
       <c r="H37">
-        <v>50.696330000000003</v>
+        <v>50.739688000000001</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38">
-        <v>727797</v>
+        <v>653501</v>
       </c>
       <c r="B38">
-        <v>727797</v>
+        <v>653501</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="E38">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F38">
-        <v>3</v>
-      </c>
-      <c r="G38" t="s">
         <v>9</v>
       </c>
+      <c r="G38">
+        <v>39.443812999999999</v>
+      </c>
       <c r="H38">
-        <v>6.1481000000000001E-2</v>
+        <v>39.443812999999999</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39">
-        <v>727849</v>
+        <v>727726</v>
       </c>
       <c r="B39">
-        <v>727849</v>
+        <v>727726</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E39">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F39">
-        <v>15</v>
-      </c>
-      <c r="G39" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G39">
+        <v>50.696330000000003</v>
       </c>
       <c r="H39">
-        <v>80.979934</v>
+        <v>50.696330000000003</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40">
-        <v>728392</v>
+        <v>1234</v>
       </c>
       <c r="B40">
-        <v>728392</v>
+        <v>1234</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="E40">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F40">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="G40">
-        <v>5.4994259999999997</v>
+        <v>46.370142000000001</v>
       </c>
       <c r="H40">
-        <v>5.4994259999999997</v>
+        <v>46.370142000000001</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41">
-        <v>100289462</v>
+        <v>727849</v>
       </c>
       <c r="B41">
-        <v>100289462</v>
+        <v>727849</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E41">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F41">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G41">
-        <v>7.4148630000000004</v>
+        <v>80.979934</v>
       </c>
       <c r="H41">
-        <v>7.4148630000000004</v>
+        <v>80.979934</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42">
-        <v>28387</v>
+        <v>728392</v>
       </c>
       <c r="B42">
-        <v>28387</v>
+        <v>728392</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E42">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F42">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G42">
-        <v>106.851112</v>
+        <v>5.4994259999999997</v>
       </c>
       <c r="H42">
-        <v>106.851112</v>
+        <v>5.4994259999999997</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43">
-        <v>94431</v>
+        <v>100289462</v>
       </c>
       <c r="B43">
-        <v>94431</v>
+        <v>100289462</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E43">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F43">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G43">
-        <v>21.715451000000002</v>
+        <v>7.4148630000000004</v>
       </c>
       <c r="H43">
-        <v>21.715451000000002</v>
+        <v>7.4148630000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44">
+        <v>91522</v>
+      </c>
+      <c r="B44">
+        <v>91522</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>5</v>
+      </c>
+      <c r="G44">
+        <v>178.237616</v>
+      </c>
+      <c r="H44">
+        <v>178.237616</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45">
+        <v>729021</v>
+      </c>
+      <c r="B45">
+        <v>729021</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <v>119.77424499999999</v>
+      </c>
+      <c r="H45">
+        <v>119.77424499999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46">
+        <v>88523</v>
+      </c>
+      <c r="B46">
+        <v>88523</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46">
+        <v>13</v>
+      </c>
+      <c r="F46">
+        <v>13</v>
+      </c>
+      <c r="G46">
+        <v>31.905007000000001</v>
+      </c>
+      <c r="H46">
+        <v>31.905007000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47">
+        <v>80216</v>
+      </c>
+      <c r="B47">
+        <v>80216</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <v>4</v>
+      </c>
+      <c r="G47">
+        <v>112.285995</v>
+      </c>
+      <c r="H47">
+        <v>112.285995</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48">
+        <v>5522</v>
+      </c>
+      <c r="B48">
+        <v>5522</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <v>4</v>
+      </c>
+      <c r="G48">
+        <v>6.3205780000000003</v>
+      </c>
+      <c r="H48">
+        <v>6.3205780000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2000,10 +2159,10 @@
         <v>283874</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>16</v>
@@ -2026,10 +2185,10 @@
         <v>285074</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2052,16 +2211,16 @@
         <v>282808</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" t="s">
         <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
       </c>
       <c r="G6">
         <v>102.93727199999999</v>
@@ -2078,10 +2237,10 @@
         <v>85452</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2104,10 +2263,10 @@
         <v>387820</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8">
         <v>11</v>
@@ -2130,10 +2289,10 @@
         <v>388022</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>14</v>
@@ -2156,10 +2315,10 @@
         <v>389833</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -2182,16 +2341,16 @@
         <v>389834</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G11">
         <v>5.1062000000000003E-2</v>
@@ -2208,10 +2367,10 @@
         <v>400464</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12">
         <v>15</v>
@@ -2234,10 +2393,10 @@
         <v>400499</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13">
         <v>16</v>
@@ -2260,10 +2419,10 @@
         <v>400924</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14">
         <v>22</v>
@@ -2286,10 +2445,10 @@
         <v>400968</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E15">
         <v>15</v>
@@ -2312,10 +2471,10 @@
         <v>401252</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16">
         <v>6</v>
@@ -2338,16 +2497,16 @@
         <v>401589</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17">
         <v>52.051169999999999</v>
@@ -2364,10 +2523,10 @@
         <v>440337</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -2390,10 +2549,10 @@
         <v>440568</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -2416,10 +2575,10 @@
         <v>440570</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -2442,10 +2601,10 @@
         <v>441070</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E21">
         <v>5</v>
@@ -2468,10 +2627,10 @@
         <v>441120</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22">
         <v>5</v>
@@ -2494,10 +2653,10 @@
         <v>441193</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23">
         <v>7</v>
@@ -2520,10 +2679,10 @@
         <v>441257</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24">
         <v>7</v>
@@ -2546,10 +2705,10 @@
         <v>441268</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E25">
         <v>7</v>
@@ -2572,10 +2731,10 @@
         <v>441956</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26">
         <v>21</v>
@@ -2598,10 +2757,10 @@
         <v>442535</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E27">
         <v>7</v>
@@ -2624,10 +2783,10 @@
         <v>541469</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E28">
         <v>19</v>
@@ -2650,10 +2809,10 @@
         <v>541473</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E29">
         <v>7</v>
@@ -2676,10 +2835,10 @@
         <v>642897</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E30">
         <v>11</v>
@@ -2702,10 +2861,10 @@
         <v>643576</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E31">
         <v>12</v>
@@ -2728,16 +2887,16 @@
         <v>644563</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G32">
         <v>107.131573</v>
@@ -2754,10 +2913,10 @@
         <v>646347</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -2780,10 +2939,10 @@
         <v>646517</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E34">
         <v>6</v>
@@ -2806,10 +2965,10 @@
         <v>727726</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E35">
         <v>10</v>
@@ -2832,10 +2991,10 @@
         <v>727849</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E36">
         <v>15</v>
@@ -2858,10 +3017,10 @@
         <v>728392</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E37">
         <v>17</v>
@@ -2884,10 +3043,10 @@
         <v>100289462</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E38">
         <v>8</v>
@@ -2910,10 +3069,10 @@
         <v>88523</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E39">
         <v>13</v>
@@ -2936,10 +3095,10 @@
         <v>90925</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E40">
         <v>14</v>
@@ -2962,10 +3121,10 @@
         <v>91431</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -3091,10 +3250,10 @@
         <v>57661</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E4">
         <v>11</v>
@@ -3117,10 +3276,10 @@
         <v>100507321</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>16</v>
@@ -3143,10 +3302,10 @@
         <v>284009</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E6">
         <v>17</v>
@@ -3169,10 +3328,10 @@
         <v>729956</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E7">
         <v>19</v>
@@ -3195,10 +3354,10 @@
         <v>285074</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -3221,16 +3380,16 @@
         <v>282808</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" t="s">
         <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
       </c>
       <c r="G9">
         <v>102.93727199999999</v>
@@ -3247,10 +3406,10 @@
         <v>8027</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E10">
         <v>10</v>
@@ -3273,10 +3432,10 @@
         <v>387720</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -3299,10 +3458,10 @@
         <v>100506127</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E12">
         <v>11</v>
@@ -3325,10 +3484,10 @@
         <v>2113</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13">
         <v>11</v>
@@ -3351,10 +3510,10 @@
         <v>388022</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14">
         <v>14</v>
@@ -3377,10 +3536,10 @@
         <v>389833</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -3403,10 +3562,10 @@
         <v>256158</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16">
         <v>9</v>
@@ -3429,10 +3588,10 @@
         <v>5046</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17">
         <v>15</v>
@@ -3455,10 +3614,10 @@
         <v>400499</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -3481,10 +3640,10 @@
         <v>400924</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E19">
         <v>22</v>
@@ -3507,10 +3666,10 @@
         <v>729857</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -3533,10 +3692,10 @@
         <v>442075</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21">
         <v>3</v>
@@ -3559,10 +3718,10 @@
         <v>401072</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -3585,10 +3744,10 @@
         <v>55750</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E23">
         <v>7</v>
@@ -3611,16 +3770,16 @@
         <v>401589</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24">
         <v>52.051169999999999</v>
@@ -3637,10 +3796,10 @@
         <v>402110</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -3663,10 +3822,10 @@
         <v>439985</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E26">
         <v>10</v>
@@ -3689,10 +3848,10 @@
         <v>54715</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E27">
         <v>16</v>
@@ -3715,10 +3874,10 @@
         <v>7709</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -3741,10 +3900,10 @@
         <v>23400</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -3767,10 +3926,10 @@
         <v>440742</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -3793,10 +3952,10 @@
         <v>441120</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E31">
         <v>5</v>
@@ -3819,10 +3978,10 @@
         <v>441233</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E32">
         <v>7</v>
@@ -3845,10 +4004,10 @@
         <v>441257</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E33">
         <v>7</v>
@@ -3871,10 +4030,10 @@
         <v>22853</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E34">
         <v>7</v>
@@ -3897,10 +4056,10 @@
         <v>441956</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E35">
         <v>21</v>
@@ -3923,10 +4082,10 @@
         <v>541469</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E36">
         <v>19</v>
@@ -3949,10 +4108,10 @@
         <v>541473</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E37">
         <v>7</v>
@@ -3975,10 +4134,10 @@
         <v>613266</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E38">
         <v>20</v>
@@ -4001,10 +4160,10 @@
         <v>23325</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E39">
         <v>12</v>
@@ -4027,10 +4186,10 @@
         <v>646347</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -4053,10 +4212,10 @@
         <v>399744</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E41">
         <v>10</v>
@@ -4079,10 +4238,10 @@
         <v>647115</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -4105,10 +4264,10 @@
         <v>727726</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E43">
         <v>10</v>
@@ -4131,10 +4290,10 @@
         <v>727797</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E44">
         <v>3</v>
@@ -4157,10 +4316,10 @@
         <v>727849</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E45">
         <v>15</v>
@@ -4183,10 +4342,10 @@
         <v>729021</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -4209,10 +4368,10 @@
         <v>88523</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E47">
         <v>13</v>
@@ -4235,10 +4394,10 @@
         <v>80216</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E48">
         <v>4</v>
@@ -4261,10 +4420,10 @@
         <v>5522</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E49">
         <v>4</v>
@@ -4293,7 +4452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0"/>
   <cols>
@@ -4390,10 +4549,10 @@
         <v>57661</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E4">
         <v>11</v>
@@ -4442,10 +4601,10 @@
         <v>100289124</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6">
         <v>9</v>
@@ -4468,10 +4627,10 @@
         <v>100507321</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>16</v>
@@ -4494,10 +4653,10 @@
         <v>284912</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8">
         <v>22</v>
@@ -4520,16 +4679,16 @@
         <v>282808</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" t="s">
         <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
       </c>
       <c r="G9">
         <v>102.93727199999999</v>
@@ -4546,10 +4705,10 @@
         <v>2782</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -4572,10 +4731,10 @@
         <v>2113</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11">
         <v>11</v>
@@ -4598,10 +4757,10 @@
         <v>389199</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -4624,10 +4783,10 @@
         <v>728524</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13">
         <v>7</v>
@@ -4650,10 +4809,10 @@
         <v>389833</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -4676,10 +4835,10 @@
         <v>392395</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E15">
         <v>9</v>
@@ -4702,10 +4861,10 @@
         <v>399900</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16">
         <v>11</v>
@@ -4728,10 +4887,10 @@
         <v>400499</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17">
         <v>16</v>
@@ -4754,10 +4913,10 @@
         <v>729857</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -4780,10 +4939,10 @@
         <v>442075</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19">
         <v>3</v>
@@ -4806,10 +4965,10 @@
         <v>401252</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20">
         <v>6</v>
@@ -4832,10 +4991,10 @@
         <v>401296</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21">
         <v>7</v>
@@ -4858,10 +5017,10 @@
         <v>401357</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E22">
         <v>7</v>
@@ -4884,10 +5043,10 @@
         <v>401433</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23">
         <v>7</v>
@@ -4910,16 +5069,16 @@
         <v>401620</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24">
         <v>151.01788400000001</v>
@@ -4936,10 +5095,10 @@
         <v>440258</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E25">
         <v>8</v>
@@ -4962,10 +5121,10 @@
         <v>54715</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E26">
         <v>16</v>
@@ -4988,10 +5147,10 @@
         <v>7709</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -5014,10 +5173,10 @@
         <v>23400</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -5040,10 +5199,10 @@
         <v>441120</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E29">
         <v>5</v>
@@ -5066,10 +5225,10 @@
         <v>441193</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E30">
         <v>7</v>
@@ -5092,10 +5251,10 @@
         <v>441257</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E31">
         <v>7</v>
@@ -5118,10 +5277,10 @@
         <v>441956</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E32">
         <v>21</v>
@@ -5144,10 +5303,10 @@
         <v>100133036</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E33">
         <v>9</v>
@@ -5170,10 +5329,10 @@
         <v>541473</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E34">
         <v>7</v>
@@ -5196,10 +5355,10 @@
         <v>613266</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E35">
         <v>20</v>
@@ -5222,16 +5381,16 @@
         <v>644563</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G36">
         <v>107.131573</v>
@@ -5248,10 +5407,10 @@
         <v>646347</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -5274,10 +5433,10 @@
         <v>399744</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E38">
         <v>10</v>
@@ -5300,10 +5459,10 @@
         <v>646517</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E39">
         <v>6</v>
@@ -5326,10 +5485,10 @@
         <v>647115</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E40">
         <v>2</v>
@@ -5352,10 +5511,10 @@
         <v>118461</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E41">
         <v>10</v>
@@ -5378,10 +5537,10 @@
         <v>727726</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E42">
         <v>10</v>
@@ -5404,10 +5563,10 @@
         <v>727797</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E43">
         <v>3</v>
@@ -5430,10 +5589,10 @@
         <v>727849</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E44">
         <v>15</v>
@@ -5456,10 +5615,10 @@
         <v>728392</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E45">
         <v>17</v>
@@ -5482,10 +5641,10 @@
         <v>100289462</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E46">
         <v>8</v>
@@ -5508,10 +5667,10 @@
         <v>90925</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E47">
         <v>14</v>
@@ -5534,10 +5693,10 @@
         <v>94431</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E48">
         <v>16</v>

</xml_diff>